<commit_message>
updates in progress to summaries across days plots
</commit_message>
<xml_diff>
--- a/data/animals.xlsx
+++ b/data/animals.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JB\github\jbreda_animal_training\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JB\github\jbreda_animal_training\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C098193-FD20-4373-A35A-DDBC503B5C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3FBC82-A52E-483C-9286-389AF19CF832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="2205" windowWidth="18000" windowHeight="9360" xr2:uid="{6533A8A6-44E6-4283-9B10-8647EC8BD946}"/>
+    <workbookView xWindow="1395" yWindow="4050" windowWidth="18225" windowHeight="15435" xr2:uid="{6533A8A6-44E6-4283-9B10-8647EC8BD946}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="34">
   <si>
     <t>animal_id</t>
   </si>
@@ -98,9 +98,6 @@
     <t>active</t>
   </si>
   <si>
-    <t>gained</t>
-  </si>
-  <si>
     <t>nan</t>
   </si>
   <si>
@@ -132,6 +129,15 @@
   </si>
   <si>
     <t>long_evans</t>
+  </si>
+  <si>
+    <t>on_citric</t>
+  </si>
+  <si>
+    <t>off_citric</t>
+  </si>
+  <si>
+    <t>pub_minimum</t>
   </si>
 </sst>
 </file>
@@ -490,22 +496,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E78FA1-F6EA-49AF-8317-F2B2D004F2C4}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="3" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="7" width="20.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="5" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="9" width="20.85546875" customWidth="1"/>
+    <col min="10" max="11" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,385 +522,511 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
       <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
         <v>19</v>
       </c>
-      <c r="J1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" s="1">
         <v>45040</v>
       </c>
       <c r="F2" s="1">
+        <v>45107</v>
+      </c>
+      <c r="G2" s="1">
         <v>45119</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2">
+      <c r="H2" s="1">
+        <v>45125</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2">
         <v>26.14</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <f>J2*0.04</f>
+        <v>1.0456000000000001</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1">
         <v>45040</v>
       </c>
       <c r="F3" s="1">
+        <v>45107</v>
+      </c>
+      <c r="G3" s="1">
         <v>45119</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3">
+      <c r="H3" s="1">
+        <v>45125</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3">
         <v>25.84</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f t="shared" ref="K3:K8" si="0">J3*0.04</f>
+        <v>1.0336000000000001</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1">
         <v>45040</v>
       </c>
       <c r="F4" s="1">
+        <v>45107</v>
+      </c>
+      <c r="G4" s="1">
         <v>45119</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4">
+      <c r="H4" s="1">
+        <v>45125</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4">
         <v>27.45</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>1.0980000000000001</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1">
         <v>45041</v>
       </c>
-      <c r="H5">
-        <v>18.96</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
+      <c r="F5" s="1">
+        <v>45114</v>
+      </c>
+      <c r="G5" s="1">
+        <v>45133</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>19.32</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>0.77280000000000004</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="1">
         <v>45041</v>
       </c>
-      <c r="H6">
-        <v>19.96</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
+      <c r="F6" s="1">
+        <v>45114</v>
+      </c>
+      <c r="G6" s="1">
+        <v>45133</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20.260000000000002</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0.81040000000000012</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="1">
         <v>45041</v>
       </c>
-      <c r="H7">
-        <v>18.22</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
+      <c r="F7" s="1">
+        <v>45114</v>
+      </c>
+      <c r="G7" s="1">
+        <v>45133</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18.46</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>0.73840000000000006</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1">
         <v>45041</v>
       </c>
-      <c r="H8">
-        <v>18.37</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
+      <c r="F8" s="1">
+        <v>45114</v>
+      </c>
+      <c r="G8" s="1">
+        <v>45133</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>18.46</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>0.73840000000000006</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E9" s="1">
         <v>45083</v>
       </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
       <c r="H9" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1">
         <v>45083</v>
       </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
       <c r="H10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E11" s="1">
         <v>45083</v>
       </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
       <c r="H11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="J11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K11" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1">
         <v>45083</v>
       </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="1">
+        <v>45121</v>
+      </c>
       <c r="H12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E13" s="1">
         <v>45083</v>
       </c>
+      <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1">
+        <v>45121</v>
+      </c>
       <c r="H13" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="K13" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1">
         <v>45083</v>
       </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" s="1">
+        <v>45121</v>
+      </c>
       <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="J14" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="K14" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>